<commit_message>
+edidAdmis, but with an error at the level listPromDet
After adding "/deleteAdmis"
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>#</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Passable</t>
+  </si>
+  <si>
+    <t>001/DEV3</t>
+  </si>
+  <si>
+    <t>001/DEV4</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +569,7 @@
     </row>
     <row r="2" spans="1:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -580,7 +586,7 @@
     </row>
     <row r="3" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -595,9 +601,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>12</v>
@@ -612,11 +618,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+    <row r="5" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>13</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="13"/>
@@ -638,8 +672,16 @@
     <hyperlink ref="C4" r:id="rId10" display="http://localhost:8080/showAdmis/3"/>
     <hyperlink ref="D4" r:id="rId11" display="http://localhost:8080/showAdmis/3"/>
     <hyperlink ref="E4" r:id="rId12" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="B5" r:id="rId13" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="B6" r:id="rId14" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="C5" r:id="rId15" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="C6" r:id="rId16" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="D5" r:id="rId17" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="D6" r:id="rId18" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="E5" r:id="rId19" display="http://localhost:8080/showAdmis/3"/>
+    <hyperlink ref="E6" r:id="rId20" display="http://localhost:8080/showAdmis/3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>